<commit_message>
Inseri gerador de usuario, ajustado algumas funcoes do projeto, retirado thread sleep.
</commit_message>
<xml_diff>
--- a/target/Excel/Dados.xlsx
+++ b/target/Excel/Dados.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matheus.vieira\Desktop\MeuProjeto\AdvShopMobileBDD\target\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matheus.vieira\Desktop\Apresentar\AdvShopMobileBDD\target\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2600371-B000-435C-9896-00AD348DF247}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDFD8656-2E63-43DA-A30D-1B95FFFA1C2E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3720" yWindow="1965" windowWidth="15375" windowHeight="7875" xr2:uid="{E0E69BFF-8C0C-4BBC-880E-E66347D52EC9}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="15375" windowHeight="7875" xr2:uid="{E0E69BFF-8C0C-4BBC-880E-E66347D52EC9}"/>
   </bookViews>
   <sheets>
     <sheet name="Contas" sheetId="1" r:id="rId1"/>
@@ -122,7 +122,7 @@
     <t>BOSE SOUNDLINK</t>
   </si>
   <si>
-    <t>LegoZ80</t>
+    <t>LegoZ86</t>
   </si>
 </sst>
 </file>

</xml_diff>